<commit_message>
excel file with image
</commit_message>
<xml_diff>
--- a/Sales/Annual_Report.xlsx
+++ b/Sales/Annual_Report.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2014" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -111,6 +111,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="571500"/>
+          <a:ext cx="3657607" cy="1828804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,5 +533,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sorted based on Profit
</commit_message>
<xml_diff>
--- a/Sales/Annual_Report.xlsx
+++ b/Sales/Annual_Report.xlsx
@@ -31,10 +31,10 @@
     <t>Board</t>
   </si>
   <si>
+    <t>Outdoor</t>
+  </si>
+  <si>
     <t>Legos</t>
-  </si>
-  <si>
-    <t>Outdoor</t>
   </si>
   <si>
     <t>Puzzles</t>
@@ -480,13 +480,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1371630</v>
+        <v>1219130</v>
       </c>
       <c r="C3">
-        <v>1531116</v>
+        <v>1324558</v>
       </c>
       <c r="D3">
-        <v>159486</v>
+        <v>105428</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -494,13 +494,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1219130</v>
+        <v>491028</v>
       </c>
       <c r="C4">
-        <v>1324558</v>
+        <v>559236</v>
       </c>
       <c r="D4">
-        <v>105428</v>
+        <v>68208</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>